<commit_message>
Add paymentReference and dealerName to the invoice entity
</commit_message>
<xml_diff>
--- a/src/test/resources/files/invoice.xlsx
+++ b/src/test/resources/files/invoice.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>2021/01/01</t>
   </si>
@@ -148,6 +148,90 @@
   </si>
   <si>
     <t>invoiceNumber13</t>
+  </si>
+  <si>
+    <t>paymentReference</t>
+  </si>
+  <si>
+    <t>paymentReference1</t>
+  </si>
+  <si>
+    <t>paymentReference2</t>
+  </si>
+  <si>
+    <t>paymentReference3</t>
+  </si>
+  <si>
+    <t>paymentReference4</t>
+  </si>
+  <si>
+    <t>paymentReference5</t>
+  </si>
+  <si>
+    <t>paymentReference6</t>
+  </si>
+  <si>
+    <t>paymentReference7</t>
+  </si>
+  <si>
+    <t>paymentReference8</t>
+  </si>
+  <si>
+    <t>paymentReference9</t>
+  </si>
+  <si>
+    <t>paymentReference10</t>
+  </si>
+  <si>
+    <t>paymentReference11</t>
+  </si>
+  <si>
+    <t>paymentReference12</t>
+  </si>
+  <si>
+    <t>paymentReference13</t>
+  </si>
+  <si>
+    <t>dealerName</t>
+  </si>
+  <si>
+    <t>dealerName1</t>
+  </si>
+  <si>
+    <t>dealerName2</t>
+  </si>
+  <si>
+    <t>dealerName3</t>
+  </si>
+  <si>
+    <t>dealerName4</t>
+  </si>
+  <si>
+    <t>dealerName5</t>
+  </si>
+  <si>
+    <t>dealerName6</t>
+  </si>
+  <si>
+    <t>dealerName7</t>
+  </si>
+  <si>
+    <t>dealerName8</t>
+  </si>
+  <si>
+    <t>dealerName9</t>
+  </si>
+  <si>
+    <t>dealerName10</t>
+  </si>
+  <si>
+    <t>dealerName11</t>
+  </si>
+  <si>
+    <t>dealerName12</t>
+  </si>
+  <si>
+    <t>dealerName13</t>
   </si>
 </sst>
 </file>
@@ -487,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +583,7 @@
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -512,8 +596,14 @@
       <c r="D1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -526,8 +616,14 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -540,8 +636,14 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -554,8 +656,14 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -568,8 +676,14 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -582,8 +696,14 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -596,8 +716,14 @@
       <c r="D7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -610,8 +736,14 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -624,8 +756,14 @@
       <c r="D9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -638,8 +776,14 @@
       <c r="D10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -652,8 +796,14 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -666,8 +816,14 @@
       <c r="D12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -680,8 +836,14 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -693,6 +855,12 @@
       </c>
       <c r="D14" t="s">
         <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>